<commit_message>
Added my track terms to Ivan's list
</commit_message>
<xml_diff>
--- a/Twitter Sentiment - Local/twitternames.xlsx
+++ b/Twitter Sentiment - Local/twitternames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Ivan\Twitter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Election Project\GitHub\Twitter Sentiment - Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="400">
   <si>
     <t>LibDem</t>
   </si>
@@ -1042,6 +1042,189 @@
   </si>
   <si>
     <t>@Tony__Cox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKIP </t>
+  </si>
+  <si>
+    <t>Constituency</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Dartford</t>
+  </si>
+  <si>
+    <t>DA1 2DF</t>
+  </si>
+  <si>
+    <t>Bachchu Kaini</t>
+  </si>
+  <si>
+    <t>@BKKaini</t>
+  </si>
+  <si>
+    <t>Gareth Johnson</t>
+  </si>
+  <si>
+    <t>Andy Blatchford</t>
+  </si>
+  <si>
+    <t>Ben Robert Fryer</t>
+  </si>
+  <si>
+    <t>Simon Beard</t>
+  </si>
+  <si>
+    <t>@Simon_Beard</t>
+  </si>
+  <si>
+    <t>Daisy Page</t>
+  </si>
+  <si>
+    <t>@DaisyPage07</t>
+  </si>
+  <si>
+    <t>Loughborough</t>
+  </si>
+  <si>
+    <t> LE11 5AL</t>
+  </si>
+  <si>
+    <t>Jewel Miah</t>
+  </si>
+  <si>
+    <t>@jewelmiah</t>
+  </si>
+  <si>
+    <t>Nicky Morgan</t>
+  </si>
+  <si>
+    <t>@NickyMorgan01</t>
+  </si>
+  <si>
+    <t>David Walker</t>
+  </si>
+  <si>
+    <t>Northampton North</t>
+  </si>
+  <si>
+    <t>NN2 7QF</t>
+  </si>
+  <si>
+    <t>Sally Keeble</t>
+  </si>
+  <si>
+    <t>@Sally_Keeble</t>
+  </si>
+  <si>
+    <t>Michael Ellis</t>
+  </si>
+  <si>
+    <t>@Michael_Ellis1</t>
+  </si>
+  <si>
+    <t>Steve Miller</t>
+  </si>
+  <si>
+    <t>@serial_miller</t>
+  </si>
+  <si>
+    <t>Portsmouth North</t>
+  </si>
+  <si>
+    <t>PO6 2QS</t>
+  </si>
+  <si>
+    <t>Rumal Khan</t>
+  </si>
+  <si>
+    <t>@RumalKhan</t>
+  </si>
+  <si>
+    <t>Penny Mordaunt</t>
+  </si>
+  <si>
+    <t>@PompeyToryParty</t>
+  </si>
+  <si>
+    <t>Darren Sanders</t>
+  </si>
+  <si>
+    <t>@darrensandersld</t>
+  </si>
+  <si>
+    <t>Watford</t>
+  </si>
+  <si>
+    <t>WD17 2LW</t>
+  </si>
+  <si>
+    <t>Chris Ostrowski</t>
+  </si>
+  <si>
+    <t>@Chris4Watford</t>
+  </si>
+  <si>
+    <t>Ian Alexander Eric Stotesbury</t>
+  </si>
+  <si>
+    <t>@ianstotesbury</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>LN1 1ES</t>
+  </si>
+  <si>
+    <t>Karen Lee</t>
+  </si>
+  <si>
+    <t>@KForCullercoats</t>
+  </si>
+  <si>
+    <t>Karl McCartney</t>
+  </si>
+  <si>
+    <t>@karlmccartney</t>
+  </si>
+  <si>
+    <t>Bristol North West</t>
+  </si>
+  <si>
+    <t>BS8 1NA</t>
+  </si>
+  <si>
+    <t>Darren Jones</t>
+  </si>
+  <si>
+    <t>@darrenpjones</t>
+  </si>
+  <si>
+    <t>Charlotte Leslie</t>
+  </si>
+  <si>
+    <t>@CharlotteLeslie</t>
+  </si>
+  <si>
+    <t>Sharmila Bousa</t>
+  </si>
+  <si>
+    <t>@sharmilabousa</t>
+  </si>
+  <si>
+    <t>Celia Downie</t>
+  </si>
+  <si>
+    <t>@CeliaBristol</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1232,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1071,6 +1254,25 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1150,7 +1352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1161,16 +1363,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1463,7 +1681,7 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1472,7 +1690,7 @@
     <col min="8" max="8" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="C1" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1729,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="C3" s="6" t="s">
         <v>83</v>
       </c>
@@ -1524,14 +1742,14 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1770,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>79</v>
@@ -1568,7 +1786,7 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1576,7 +1794,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1597,7 +1815,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
         <v>77</v>
@@ -1613,7 +1831,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" s="1"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1621,7 +1839,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1856,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="C12" s="3"/>
       <c r="D12" s="6" t="s">
         <v>75</v>
@@ -1646,13 +1864,13 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="C13" s="4"/>
       <c r="D13" s="6"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1669,7 +1887,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" s="1"/>
       <c r="C15" s="6" t="s">
         <v>73</v>
@@ -1680,14 +1898,14 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1706,7 +1924,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="B18" s="1"/>
       <c r="C18" s="6" t="s">
         <v>71</v>
@@ -1718,7 +1936,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1726,7 +1944,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1967,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="B21" s="1"/>
       <c r="C21" s="6" t="s">
         <v>68</v>
@@ -1767,7 +1985,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="B22" s="1"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1775,7 +1993,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1794,7 +2012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="B24" s="1"/>
       <c r="C24" s="6" t="s">
         <v>66</v>
@@ -1805,14 +2023,14 @@
       <c r="G24" s="4"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="B25" s="1"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1833,7 +2051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="B27" s="1"/>
       <c r="C27" s="6" t="s">
         <v>61</v>
@@ -1848,14 +2066,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="B28" s="1"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +2095,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="C30" t="s">
         <v>59</v>
       </c>
@@ -1922,13 +2140,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
@@ -1948,7 +2166,7 @@
     <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="B1" t="s">
         <v>89</v>
       </c>
@@ -1992,7 +2210,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2043,7 +2261,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="B3" t="s">
         <v>100</v>
       </c>
@@ -2094,7 +2312,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="B4" t="s">
         <v>100</v>
       </c>
@@ -2110,12 +2328,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="J5" s="11"/>
       <c r="K5" s="10"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2166,7 +2384,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="B7" t="s">
         <v>110</v>
       </c>
@@ -2214,7 +2432,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="B8" t="s">
         <v>110</v>
       </c>
@@ -2230,12 +2448,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="J9" s="11"/>
       <c r="K9" s="10"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2286,7 +2504,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="B11" t="s">
         <v>116</v>
       </c>
@@ -2335,7 +2553,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="B12" t="s">
         <v>116</v>
       </c>
@@ -2351,12 +2569,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="J13" s="11"/>
       <c r="K13" s="10"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2407,7 +2625,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -2455,7 +2673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -2471,7 +2689,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -2485,7 +2703,7 @@
       </c>
       <c r="P17" s="13"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -2501,12 +2719,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="J19" s="11"/>
       <c r="K19" s="10"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>5</v>
       </c>
@@ -2557,7 +2775,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>124</v>
       </c>
@@ -2608,11 +2826,11 @@
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="J22" s="11"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2663,7 +2881,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="B24" t="s">
         <v>131</v>
       </c>
@@ -2711,7 +2929,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="B25" t="s">
         <v>131</v>
       </c>
@@ -2727,7 +2945,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="B26" t="s">
         <v>131</v>
       </c>
@@ -2741,11 +2959,11 @@
       </c>
       <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="J27" s="11"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>7</v>
       </c>
@@ -2796,7 +3014,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="B29" t="s">
         <v>134</v>
       </c>
@@ -2847,7 +3065,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="B30" t="s">
         <v>134</v>
       </c>
@@ -2863,7 +3081,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="J31" s="11"/>
       <c r="K31" s="10"/>
       <c r="O31" t="str">
@@ -2871,7 +3089,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>8</v>
       </c>
@@ -2922,7 +3140,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="B33" t="s">
         <v>4</v>
       </c>
@@ -2970,7 +3188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -2986,7 +3204,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="J35" s="11"/>
       <c r="K35" s="10"/>
       <c r="O35" t="str">
@@ -2994,7 +3212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>9</v>
       </c>
@@ -3045,7 +3263,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="B37" t="s">
         <v>143</v>
       </c>
@@ -3093,7 +3311,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="B38" t="s">
         <v>143</v>
       </c>
@@ -3109,7 +3327,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="J39" s="11"/>
       <c r="K39" s="10"/>
       <c r="O39" t="str">
@@ -3117,7 +3335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>10</v>
       </c>
@@ -3168,7 +3386,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="B41" t="s">
         <v>147</v>
       </c>
@@ -3219,7 +3437,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="B42" t="s">
         <v>147</v>
       </c>
@@ -3233,11 +3451,11 @@
       </c>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="J43" s="11"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>11</v>
       </c>
@@ -3288,7 +3506,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="B45" t="s">
         <v>152</v>
       </c>
@@ -3339,11 +3557,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="J46" s="11"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>12</v>
       </c>
@@ -3394,7 +3612,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="B48" t="s">
         <v>158</v>
       </c>
@@ -3445,7 +3663,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="B49" t="s">
         <v>158</v>
       </c>
@@ -3459,7 +3677,7 @@
       </c>
       <c r="P49" s="13"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="B50" t="s">
         <v>158</v>
       </c>
@@ -3473,11 +3691,11 @@
       </c>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="J51" s="11"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>13</v>
       </c>
@@ -3528,7 +3746,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="B53" t="s">
         <v>163</v>
       </c>
@@ -3576,7 +3794,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="B54" t="s">
         <v>163</v>
       </c>
@@ -3592,7 +3810,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="B55" t="s">
         <v>163</v>
       </c>
@@ -3606,11 +3824,11 @@
       </c>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="J56" s="11"/>
       <c r="K56" s="10"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="A57">
         <v>14</v>
       </c>
@@ -3661,7 +3879,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="B58" t="s">
         <v>168</v>
       </c>
@@ -3709,7 +3927,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="B59" t="s">
         <v>168</v>
       </c>
@@ -3722,7 +3940,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="B60" t="s">
         <v>168</v>
       </c>
@@ -3735,11 +3953,11 @@
         <v>308</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="J61" s="11"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16">
       <c r="A62">
         <v>15</v>
       </c>
@@ -3786,7 +4004,7 @@
       </c>
       <c r="P62" s="13"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="B63" t="s">
         <v>173</v>
       </c>
@@ -3832,11 +4050,11 @@
       </c>
       <c r="P63" s="13"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="J64" s="11"/>
       <c r="K64" s="10"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65">
         <v>16</v>
       </c>
@@ -3887,7 +4105,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="B66" t="s">
         <v>182</v>
       </c>
@@ -3938,7 +4156,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="B67" t="s">
         <v>182</v>
       </c>
@@ -3951,11 +4169,11 @@
         <v>312</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="J68" s="11"/>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69">
         <v>17</v>
       </c>
@@ -4006,7 +4224,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="B70" t="s">
         <v>187</v>
       </c>
@@ -4052,11 +4270,11 @@
       </c>
       <c r="P70" s="13"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="J71" s="11"/>
       <c r="K71" s="10"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72">
         <v>18</v>
       </c>
@@ -4107,7 +4325,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="B73" t="s">
         <v>192</v>
       </c>
@@ -4155,7 +4373,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="B74" t="s">
         <v>192</v>
       </c>
@@ -4171,7 +4389,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="B75" t="s">
         <v>192</v>
       </c>
@@ -4187,11 +4405,11 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="J76" s="11"/>
       <c r="K76" s="10"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77">
         <v>19</v>
       </c>
@@ -4240,7 +4458,7 @@
       </c>
       <c r="P77" s="15"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="B78" t="s">
         <v>199</v>
       </c>
@@ -4288,15 +4506,15 @@
         <v>338</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="J79" s="11"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17">
       <c r="J80" s="11"/>
       <c r="K80" s="10"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="A81">
         <v>20</v>
       </c>
@@ -4344,7 +4562,7 @@
         <v>Simon Kirby</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="B82" t="s">
         <v>204</v>
       </c>
@@ -4389,15 +4607,15 @@
         <v>Nancy Platts</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="J83" s="11"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="J84" s="11"/>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16">
       <c r="A85">
         <v>21</v>
       </c>
@@ -4448,7 +4666,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="B86" t="s">
         <v>209</v>
       </c>
@@ -4493,15 +4711,15 @@
         <v>David Wright</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16">
       <c r="J87" s="11"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16">
       <c r="J88" s="11"/>
       <c r="K88" s="10"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16">
       <c r="A89">
         <v>22</v>
       </c>
@@ -4552,7 +4770,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16">
       <c r="B90" t="s">
         <v>213</v>
       </c>
@@ -4600,7 +4818,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="B91" t="s">
         <v>213</v>
       </c>
@@ -4616,11 +4834,11 @@
         <v>324</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="J92" s="11"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="A93">
         <v>23</v>
       </c>
@@ -4671,7 +4889,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16">
       <c r="B94" t="s">
         <v>217</v>
       </c>
@@ -4719,7 +4937,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16">
       <c r="B95" t="s">
         <v>217</v>
       </c>
@@ -4735,7 +4953,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="B96" t="s">
         <v>217</v>
       </c>
@@ -4751,11 +4969,11 @@
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="J97" s="11"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="A98">
         <v>24</v>
       </c>
@@ -4803,7 +5021,7 @@
         <v>David Mundell</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="B99" t="s">
         <v>220</v>
       </c>
@@ -4848,11 +5066,11 @@
         <v>Emma Harper</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17">
       <c r="J100" s="11"/>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101">
         <v>25</v>
       </c>
@@ -4903,7 +5121,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17">
       <c r="B102" t="s">
         <v>224</v>
       </c>
@@ -4951,11 +5169,11 @@
         <v>333</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17">
       <c r="J103" s="11"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17">
       <c r="A104">
         <v>26</v>
       </c>
@@ -5009,7 +5227,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17">
       <c r="B105" t="s">
         <v>225</v>
       </c>
@@ -5057,7 +5275,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17">
       <c r="B106" t="s">
         <v>225</v>
       </c>
@@ -5071,7 +5289,7 @@
       </c>
       <c r="P106" s="12"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17">
       <c r="A108">
         <v>27</v>
       </c>
@@ -5119,7 +5337,7 @@
         <v>Graham Evans</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17">
       <c r="B109" t="s">
         <v>231</v>
       </c>
@@ -5164,11 +5382,11 @@
         <v>Julia Tickridge</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17">
       <c r="J110" s="11"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17">
       <c r="B111" s="17" t="s">
         <v>235</v>
       </c>
@@ -5213,7 +5431,7 @@
         <v>Alistair Carmichael</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17">
       <c r="B112" s="17" t="s">
         <v>235</v>
       </c>
@@ -5258,7 +5476,7 @@
         <v>Danus  Skene</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:15">
       <c r="B113" s="17" t="s">
         <v>240</v>
       </c>
@@ -5303,7 +5521,7 @@
         <v>Alasdair McDonnell</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:15">
       <c r="B114" s="17" t="s">
         <v>240</v>
       </c>
@@ -5348,7 +5566,7 @@
         <v>Jonathan Bell</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:15">
       <c r="B115" s="17" t="s">
         <v>249</v>
       </c>
@@ -5391,7 +5609,7 @@
         <v>Danny Kinahan</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:15">
       <c r="B116" s="17" t="s">
         <v>249</v>
       </c>
@@ -5436,7 +5654,300 @@
         <v>William McCrea</v>
       </c>
     </row>
+    <row r="119" spans="2:15">
+      <c r="B119" s="20"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G119" s="21"/>
+      <c r="H119" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I119" s="21"/>
+      <c r="J119" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="K119" s="21"/>
+      <c r="L119" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M119" s="21"/>
+    </row>
+    <row r="120" spans="2:15">
+      <c r="B120" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="C120" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E120" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="F120" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="G120" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H120" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="I120" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="J120" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="K120" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="L120" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="M120" s="20" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="121" spans="2:15">
+      <c r="B121" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C121" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="E121" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="F121" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="G121" s="23"/>
+      <c r="H121" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="I121" s="23"/>
+      <c r="J121" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="K121" s="23"/>
+      <c r="L121" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="M121" s="22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="122" spans="2:15">
+      <c r="B122" s="20"/>
+      <c r="C122" s="20"/>
+      <c r="D122" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="E122" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="F122" s="22"/>
+      <c r="G122" s="22"/>
+      <c r="H122" s="22"/>
+      <c r="I122" s="22"/>
+      <c r="J122" s="22"/>
+      <c r="K122" s="22"/>
+      <c r="L122" s="22"/>
+      <c r="M122" s="22"/>
+    </row>
+    <row r="123" spans="2:15">
+      <c r="B123" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="C123" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="D123" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="E123" t="s">
+        <v>358</v>
+      </c>
+      <c r="F123" t="s">
+        <v>359</v>
+      </c>
+      <c r="G123" t="s">
+        <v>360</v>
+      </c>
+      <c r="H123" s="22"/>
+      <c r="I123" s="22"/>
+      <c r="J123" s="22"/>
+      <c r="K123" s="22"/>
+      <c r="L123" t="s">
+        <v>361</v>
+      </c>
+      <c r="M123" s="23"/>
+    </row>
+    <row r="124" spans="2:15">
+      <c r="B124" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="C124" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="D124" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="E124" t="s">
+        <v>365</v>
+      </c>
+      <c r="F124" t="s">
+        <v>366</v>
+      </c>
+      <c r="G124" t="s">
+        <v>367</v>
+      </c>
+      <c r="H124" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="I124" t="s">
+        <v>369</v>
+      </c>
+      <c r="J124" s="22"/>
+      <c r="K124" s="22"/>
+      <c r="L124" s="22"/>
+      <c r="M124" s="20"/>
+    </row>
+    <row r="125" spans="2:15">
+      <c r="B125" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="D125" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="E125" t="s">
+        <v>373</v>
+      </c>
+      <c r="F125" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="G125" t="s">
+        <v>375</v>
+      </c>
+      <c r="H125" s="22"/>
+      <c r="I125" s="22"/>
+      <c r="J125" s="22"/>
+      <c r="K125" s="22"/>
+      <c r="L125" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="M125" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="126" spans="2:15">
+      <c r="B126" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C126" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="D126" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="E126" t="s">
+        <v>381</v>
+      </c>
+      <c r="F126" s="22"/>
+      <c r="G126" s="22"/>
+      <c r="H126" s="22"/>
+      <c r="I126" s="22"/>
+      <c r="J126" s="22"/>
+      <c r="K126" s="22"/>
+      <c r="L126" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="M126" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="127" spans="2:15">
+      <c r="B127" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D127" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="E127" t="s">
+        <v>387</v>
+      </c>
+      <c r="F127" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="G127" t="s">
+        <v>389</v>
+      </c>
+      <c r="H127" s="22"/>
+      <c r="I127" s="22"/>
+      <c r="J127" s="22"/>
+      <c r="K127" s="22"/>
+      <c r="L127" s="27"/>
+      <c r="M127" s="27"/>
+    </row>
+    <row r="128" spans="2:15">
+      <c r="B128" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="D128" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="E128" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="F128" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="G128" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="H128" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="I128" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="J128" s="22"/>
+      <c r="K128" s="22"/>
+      <c r="L128" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="M128" s="22" t="s">
+        <v>399</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="F119:G119"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="L119:M119"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" tooltip="Byron Davies's Twitter profile" display="https://twitter.com/Byron_Davies"/>
     <hyperlink ref="P3" r:id="rId2" tooltip="Tonia Antoniazzi's Twitter profile" display="https://twitter.com/ToniaAntoniazzi"/>

</xml_diff>

<commit_message>
Updated polls, track terms for constituencies, and uploaded planning document
</commit_message>
<xml_diff>
--- a/Twitter Sentiment - Local/twitternames.xlsx
+++ b/Twitter Sentiment - Local/twitternames.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Brexit" sheetId="2" r:id="rId1"/>
     <sheet name="Margins" sheetId="3" r:id="rId2"/>
+    <sheet name="List of Constituencies" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="404">
   <si>
     <t>LibDem</t>
   </si>
@@ -1225,6 +1226,18 @@
   </si>
   <si>
     <t>@CeliaBristol</t>
+  </si>
+  <si>
+    <t>Brexit</t>
+  </si>
+  <si>
+    <t>Consistent voting</t>
+  </si>
+  <si>
+    <t>Small winning margin</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1290,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1338,6 +1351,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1352,7 +1377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1374,9 +1399,6 @@
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1389,15 +1411,40 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFDC3124"/>
     </mruColors>
   </colors>
@@ -1678,7 +1725,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2142,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="J131" sqref="J131"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5657,26 +5704,26 @@
     <row r="119" spans="2:15">
       <c r="B119" s="20"/>
       <c r="C119" s="20"/>
-      <c r="D119" s="21" t="s">
+      <c r="D119" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21" t="s">
+      <c r="E119" s="27"/>
+      <c r="F119" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G119" s="21"/>
-      <c r="H119" s="21" t="s">
+      <c r="G119" s="27"/>
+      <c r="H119" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I119" s="21"/>
-      <c r="J119" s="21" t="s">
+      <c r="I119" s="27"/>
+      <c r="J119" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="K119" s="21"/>
-      <c r="L119" s="21" t="s">
+      <c r="K119" s="27"/>
+      <c r="L119" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="M119" s="21"/>
+      <c r="M119" s="27"/>
     </row>
     <row r="120" spans="2:15">
       <c r="B120" s="20" t="s">
@@ -5723,48 +5770,51 @@
       <c r="C121" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="D121" s="22" t="s">
+      <c r="D121" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="E121" s="22" t="s">
+      <c r="E121" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="F121" s="22" t="s">
+      <c r="F121" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="G121" s="23"/>
-      <c r="H121" s="22" t="s">
+      <c r="G121" s="22"/>
+      <c r="H121" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="I121" s="23"/>
-      <c r="J121" s="22" t="s">
+      <c r="I121" s="22"/>
+      <c r="J121" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="K121" s="23"/>
-      <c r="L121" s="22" t="s">
+      <c r="K121" s="22"/>
+      <c r="L121" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="M121" s="22" t="s">
+      <c r="M121" s="21" t="s">
         <v>352</v>
+      </c>
+      <c r="O121" s="15" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="122" spans="2:15">
       <c r="B122" s="20"/>
       <c r="C122" s="20"/>
-      <c r="D122" s="22" t="s">
+      <c r="D122" s="21" t="s">
         <v>353</v>
       </c>
-      <c r="E122" s="22" t="s">
+      <c r="E122" s="21" t="s">
         <v>354</v>
       </c>
-      <c r="F122" s="22"/>
-      <c r="G122" s="22"/>
-      <c r="H122" s="22"/>
-      <c r="I122" s="22"/>
-      <c r="J122" s="22"/>
-      <c r="K122" s="22"/>
-      <c r="L122" s="22"/>
-      <c r="M122" s="22"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="21"/>
+      <c r="H122" s="21"/>
+      <c r="I122" s="21"/>
+      <c r="J122" s="21"/>
+      <c r="K122" s="21"/>
+      <c r="L122" s="21"/>
+      <c r="M122" s="21"/>
     </row>
     <row r="123" spans="2:15">
       <c r="B123" s="20" t="s">
@@ -5773,7 +5823,7 @@
       <c r="C123" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="D123" s="22" t="s">
+      <c r="D123" s="21" t="s">
         <v>357</v>
       </c>
       <c r="E123" t="s">
@@ -5785,23 +5835,23 @@
       <c r="G123" t="s">
         <v>360</v>
       </c>
-      <c r="H123" s="22"/>
-      <c r="I123" s="22"/>
-      <c r="J123" s="22"/>
-      <c r="K123" s="22"/>
+      <c r="H123" s="21"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="21"/>
+      <c r="K123" s="21"/>
       <c r="L123" t="s">
         <v>361</v>
       </c>
-      <c r="M123" s="23"/>
+      <c r="M123" s="22"/>
     </row>
     <row r="124" spans="2:15">
-      <c r="B124" s="24" t="s">
+      <c r="B124" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="C124" s="25" t="s">
+      <c r="C124" s="24" t="s">
         <v>363</v>
       </c>
-      <c r="D124" s="22" t="s">
+      <c r="D124" s="21" t="s">
         <v>364</v>
       </c>
       <c r="E124" t="s">
@@ -5813,41 +5863,41 @@
       <c r="G124" t="s">
         <v>367</v>
       </c>
-      <c r="H124" s="22" t="s">
+      <c r="H124" s="21" t="s">
         <v>368</v>
       </c>
       <c r="I124" t="s">
         <v>369</v>
       </c>
-      <c r="J124" s="22"/>
-      <c r="K124" s="22"/>
-      <c r="L124" s="22"/>
+      <c r="J124" s="21"/>
+      <c r="K124" s="21"/>
+      <c r="L124" s="21"/>
       <c r="M124" s="20"/>
     </row>
     <row r="125" spans="2:15">
-      <c r="B125" s="24" t="s">
+      <c r="B125" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="C125" s="24" t="s">
+      <c r="C125" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="D125" s="22" t="s">
+      <c r="D125" s="21" t="s">
         <v>372</v>
       </c>
       <c r="E125" t="s">
         <v>373</v>
       </c>
-      <c r="F125" s="22" t="s">
+      <c r="F125" s="21" t="s">
         <v>374</v>
       </c>
       <c r="G125" t="s">
         <v>375</v>
       </c>
-      <c r="H125" s="22"/>
-      <c r="I125" s="22"/>
-      <c r="J125" s="22"/>
-      <c r="K125" s="22"/>
-      <c r="L125" s="22" t="s">
+      <c r="H125" s="21"/>
+      <c r="I125" s="21"/>
+      <c r="J125" s="21"/>
+      <c r="K125" s="21"/>
+      <c r="L125" s="21" t="s">
         <v>376</v>
       </c>
       <c r="M125" t="s">
@@ -5855,25 +5905,25 @@
       </c>
     </row>
     <row r="126" spans="2:15">
-      <c r="B126" s="24" t="s">
+      <c r="B126" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="C126" s="24" t="s">
+      <c r="C126" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="D126" s="22" t="s">
+      <c r="D126" s="21" t="s">
         <v>380</v>
       </c>
       <c r="E126" t="s">
         <v>381</v>
       </c>
-      <c r="F126" s="22"/>
-      <c r="G126" s="22"/>
-      <c r="H126" s="22"/>
-      <c r="I126" s="22"/>
-      <c r="J126" s="22"/>
-      <c r="K126" s="22"/>
-      <c r="L126" s="22" t="s">
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="21"/>
+      <c r="J126" s="21"/>
+      <c r="K126" s="21"/>
+      <c r="L126" s="21" t="s">
         <v>382</v>
       </c>
       <c r="M126" t="s">
@@ -5881,62 +5931,62 @@
       </c>
     </row>
     <row r="127" spans="2:15">
-      <c r="B127" s="24" t="s">
+      <c r="B127" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="C127" s="26" t="s">
+      <c r="C127" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="D127" s="22" t="s">
+      <c r="D127" s="21" t="s">
         <v>386</v>
       </c>
       <c r="E127" t="s">
         <v>387</v>
       </c>
-      <c r="F127" s="22" t="s">
+      <c r="F127" s="21" t="s">
         <v>388</v>
       </c>
       <c r="G127" t="s">
         <v>389</v>
       </c>
-      <c r="H127" s="22"/>
-      <c r="I127" s="22"/>
-      <c r="J127" s="22"/>
-      <c r="K127" s="22"/>
-      <c r="L127" s="27"/>
-      <c r="M127" s="27"/>
+      <c r="H127" s="21"/>
+      <c r="I127" s="21"/>
+      <c r="J127" s="21"/>
+      <c r="K127" s="21"/>
+      <c r="L127" s="26"/>
+      <c r="M127" s="26"/>
     </row>
     <row r="128" spans="2:15">
-      <c r="B128" s="24" t="s">
+      <c r="B128" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="C128" s="26" t="s">
+      <c r="C128" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="D128" s="22" t="s">
+      <c r="D128" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="E128" s="22" t="s">
+      <c r="E128" s="21" t="s">
         <v>393</v>
       </c>
-      <c r="F128" s="22" t="s">
+      <c r="F128" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="G128" s="22" t="s">
+      <c r="G128" s="21" t="s">
         <v>395</v>
       </c>
-      <c r="H128" s="22" t="s">
+      <c r="H128" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="I128" s="22" t="s">
+      <c r="I128" s="21" t="s">
         <v>397</v>
       </c>
-      <c r="J128" s="22"/>
-      <c r="K128" s="22"/>
-      <c r="L128" s="22" t="s">
+      <c r="J128" s="21"/>
+      <c r="K128" s="21"/>
+      <c r="L128" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="M128" s="22" t="s">
+      <c r="M128" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -6008,4 +6058,306 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q6:Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="35">
+        <v>10</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="G1" s="35">
+        <v>29</v>
+      </c>
+      <c r="H1"/>
+      <c r="J1" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="K1" s="29">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="N4" s="20"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="F12" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="F13" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="F14" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="F15" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="F16" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="6:18">
+      <c r="F17" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="6:18">
+      <c r="F18" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="6:18">
+      <c r="F19" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="6:18">
+      <c r="F20" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="6:18">
+      <c r="F21" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="6:18">
+      <c r="F22" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="6:18">
+      <c r="F23" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="6:18">
+      <c r="F24" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="6:18">
+      <c r="F25" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="6:18">
+      <c r="F26" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="6:18">
+      <c r="F27" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="6:18">
+      <c r="F28" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="6:18">
+      <c r="F29" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="6:18">
+      <c r="F30" s="34" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="41" spans="5:8">
+      <c r="H41" s="30"/>
+    </row>
+    <row r="42" spans="5:8">
+      <c r="H42" s="30"/>
+    </row>
+    <row r="43" spans="5:8">
+      <c r="H43" s="30"/>
+    </row>
+    <row r="44" spans="5:8">
+      <c r="H44" s="31"/>
+    </row>
+    <row r="45" spans="5:8">
+      <c r="H45" s="31"/>
+    </row>
+    <row r="46" spans="5:8">
+      <c r="E46" s="23"/>
+      <c r="H46" s="31"/>
+    </row>
+    <row r="47" spans="5:8">
+      <c r="E47" s="23"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="5:8">
+      <c r="E48" s="23"/>
+      <c r="H48" s="31"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="23"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G1 B1 H2:H10 H40:H1048576 R2:R29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reduced the number of constituencies from 45 to 21
</commit_message>
<xml_diff>
--- a/Twitter Sentiment - Local/twitternames.xlsx
+++ b/Twitter Sentiment - Local/twitternames.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Brexit" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="408">
   <si>
     <t>LibDem</t>
   </si>
@@ -1238,6 +1238,18 @@
   </si>
   <si>
     <t>REJECTED</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Maybe reject as they don't all have twitter accounts</t>
+  </si>
+  <si>
+    <t>One Person</t>
+  </si>
+  <si>
+    <t>Four people</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1411,9 +1423,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1422,8 +1431,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1724,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2189,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5704,26 +5722,26 @@
     <row r="119" spans="2:15">
       <c r="B119" s="20"/>
       <c r="C119" s="20"/>
-      <c r="D119" s="27" t="s">
+      <c r="D119" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="E119" s="27"/>
-      <c r="F119" s="27" t="s">
+      <c r="E119" s="34"/>
+      <c r="F119" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G119" s="27"/>
-      <c r="H119" s="27" t="s">
+      <c r="G119" s="34"/>
+      <c r="H119" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I119" s="27"/>
-      <c r="J119" s="27" t="s">
+      <c r="I119" s="34"/>
+      <c r="J119" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="K119" s="27"/>
-      <c r="L119" s="27" t="s">
+      <c r="K119" s="34"/>
+      <c r="L119" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="M119" s="27"/>
+      <c r="M119" s="34"/>
     </row>
     <row r="120" spans="2:15">
       <c r="B120" s="20" t="s">
@@ -6064,297 +6082,365 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q6:Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>400</v>
       </c>
-      <c r="B1" s="35">
+      <c r="B1" s="33">
         <v>10</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="G1" s="35">
-        <v>29</v>
+      <c r="G1" s="33">
+        <v>4</v>
       </c>
       <c r="H1"/>
       <c r="J1" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="K1" s="29">
+      <c r="K1" s="28">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="28">
         <v>6</v>
       </c>
-      <c r="AA1" s="29">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="39" t="s">
         <v>355</v>
       </c>
+      <c r="K2" t="s">
+        <v>406</v>
+      </c>
       <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="27" t="s">
         <v>362</v>
       </c>
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="G4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>370</v>
       </c>
       <c r="N4" s="20"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="B5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="27" t="s">
         <v>378</v>
       </c>
       <c r="N5" s="20"/>
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="G6" s="37" t="s">
+        <v>404</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>384</v>
       </c>
       <c r="N6" s="23"/>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="B7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F7" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="G7" s="37"/>
+      <c r="J7" s="27" t="s">
         <v>390</v>
       </c>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="B8" t="s">
+        <v>406</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>143</v>
       </c>
+      <c r="G8" s="37"/>
+      <c r="J8" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="K8" t="s">
+        <v>407</v>
+      </c>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="B9" t="s">
+        <v>406</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>147</v>
       </c>
+      <c r="G9" s="37"/>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="36" t="s">
         <v>152</v>
       </c>
+      <c r="G10" s="37"/>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="B11" t="s">
+        <v>406</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>158</v>
       </c>
+      <c r="G11" s="37"/>
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="36" t="s">
         <v>163</v>
       </c>
+      <c r="G12" s="37"/>
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="36" t="s">
         <v>168</v>
       </c>
+      <c r="G13" s="37"/>
       <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="36" t="s">
         <v>173</v>
       </c>
+      <c r="G14" s="37"/>
       <c r="R14" s="4"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="36" t="s">
         <v>182</v>
       </c>
+      <c r="G15" s="37"/>
       <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:27">
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="36" t="s">
         <v>187</v>
       </c>
+      <c r="G16" s="37"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="6:18">
-      <c r="F17" s="33" t="s">
+    <row r="17" spans="1:18">
+      <c r="F17" s="36" t="s">
         <v>192</v>
       </c>
+      <c r="G17" s="37"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="6:18">
-      <c r="F18" s="33" t="s">
+    <row r="18" spans="1:18">
+      <c r="F18" s="36" t="s">
         <v>199</v>
       </c>
+      <c r="G18" s="37"/>
+      <c r="J18" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="6:18">
-      <c r="F19" s="33" t="s">
+    <row r="19" spans="1:18">
+      <c r="A19"/>
+      <c r="F19" s="36" t="s">
         <v>204</v>
       </c>
+      <c r="G19" s="37"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="6:18">
-      <c r="F20" s="33" t="s">
+    <row r="20" spans="1:18">
+      <c r="A20"/>
+      <c r="F20" s="36" t="s">
         <v>209</v>
       </c>
+      <c r="G20" s="37"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="6:18">
-      <c r="F21" s="33" t="s">
+    <row r="21" spans="1:18">
+      <c r="A21"/>
+      <c r="F21" s="36" t="s">
         <v>213</v>
       </c>
+      <c r="G21" s="37"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="6:18">
-      <c r="F22" s="33" t="s">
+    <row r="22" spans="1:18">
+      <c r="A22"/>
+      <c r="F22" s="36" t="s">
         <v>217</v>
       </c>
+      <c r="G22" s="37"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="6:18">
-      <c r="F23" s="33" t="s">
+    <row r="23" spans="1:18">
+      <c r="F23" s="36" t="s">
         <v>220</v>
       </c>
+      <c r="G23" s="37"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="6:18">
-      <c r="F24" s="33" t="s">
+    <row r="24" spans="1:18">
+      <c r="F24" s="36" t="s">
         <v>224</v>
       </c>
+      <c r="G24" s="37"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="6:18">
-      <c r="F25" s="33" t="s">
+    <row r="25" spans="1:18">
+      <c r="F25" s="36" t="s">
         <v>225</v>
       </c>
+      <c r="G25" s="37"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="6:18">
-      <c r="F26" s="33" t="s">
+    <row r="26" spans="1:18">
+      <c r="F26" s="36" t="s">
         <v>231</v>
       </c>
+      <c r="G26" s="37"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="6:18">
-      <c r="F27" s="33" t="s">
+    <row r="27" spans="1:18">
+      <c r="F27" s="36" t="s">
         <v>235</v>
       </c>
+      <c r="G27" s="37"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="6:18">
-      <c r="F28" s="33" t="s">
+    <row r="28" spans="1:18">
+      <c r="F28" s="36" t="s">
         <v>240</v>
       </c>
+      <c r="G28" s="37"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="6:18">
-      <c r="F29" s="33" t="s">
+    <row r="29" spans="1:18">
+      <c r="F29" s="36" t="s">
         <v>249</v>
       </c>
+      <c r="G29" s="37"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="6:18">
-      <c r="F30" s="34" t="s">
-        <v>340</v>
-      </c>
+    <row r="30" spans="1:18">
+      <c r="F30" s="29"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="41" spans="5:8">
-      <c r="H41" s="30"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="5:8">
-      <c r="H42" s="30"/>
+      <c r="H42" s="29"/>
     </row>
     <row r="43" spans="5:8">
-      <c r="H43" s="30"/>
+      <c r="H43" s="29"/>
     </row>
     <row r="44" spans="5:8">
-      <c r="H44" s="31"/>
+      <c r="H44" s="30"/>
     </row>
     <row r="45" spans="5:8">
-      <c r="H45" s="31"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" spans="5:8">
       <c r="E46" s="23"/>
-      <c r="H46" s="31"/>
+      <c r="H46" s="30"/>
     </row>
     <row r="47" spans="5:8">
       <c r="E47" s="23"/>
-      <c r="H47" s="31"/>
+      <c r="H47" s="30"/>
     </row>
     <row r="48" spans="5:8">
       <c r="E48" s="23"/>
-      <c r="H48" s="31"/>
+      <c r="H48" s="30"/>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G6:G30"/>
+  </mergeCells>
   <conditionalFormatting sqref="G1 B1 H2:H10 H40:H1048576 R2:R29">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>